<commit_message>
feat(formulaire): updated ligne-formulaire update to delete links to formulaire.
</commit_message>
<xml_diff>
--- a/src/main/resources/static/templates/formulaires.xlsx
+++ b/src/main/resources/static/templates/formulaires.xlsx
@@ -1,23 +1,156 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="J4")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="formulaires", var="formulaire", multisheet="sheetNames")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="formulaire.sections", var="section")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="section.sections" var="section")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+  <si>
+    <t>Questionnaire</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Libelle</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>$(formulaire.name)</t>
+  </si>
+  <si>
+    <t>$(formulaire.numero)</t>
+  </si>
+  <si>
+    <t>$(section.name)</t>
+  </si>
+  <si>
+    <t>$(section.ordre)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +158,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -42,23 +194,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -343,37 +540,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>